<commit_message>
added plots for stare scans
</commit_message>
<xml_diff>
--- a/configs/lidargo/config_examples_stand.xlsx
+++ b/configs/lidargo/config_examples_stand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SLETIZIA\OneDrive - NREL\Desktop\PostDoc\Software\FIEXTA\configs\lidargo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72598104-448F-4CE7-9C98-3BF65493D107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C591812B-4441-44B7-AB8C-836FFDC62E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2124" yWindow="7644" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -641,21 +641,21 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H2" sqref="H2"/>
+      <selection pane="topRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="5" max="5" width="47.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -675,7 +675,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -695,7 +695,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -715,7 +715,7 @@
         <v>20230101</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -735,7 +735,7 @@
         <v>20240101</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,7 +755,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -796,7 +796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -816,7 +816,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -836,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>2</v>
       </c>
@@ -856,7 +856,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -876,7 +876,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -896,7 +896,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -916,7 +916,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
@@ -930,13 +930,13 @@
         <v>0.25</v>
       </c>
       <c r="E14" s="19">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="F14" s="19">
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
@@ -956,7 +956,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
@@ -976,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>9</v>
       </c>
@@ -996,7 +996,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>10</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>11</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>12</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1166,7 +1166,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>20</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>22</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>23</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>24</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>25</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>26</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
final graphic tweaks and full testing
</commit_message>
<xml_diff>
--- a/configs/lidargo/config_examples_stand.xlsx
+++ b/configs/lidargo/config_examples_stand.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SLETIZIA\OneDrive - NREL\Desktop\PostDoc\Software\FIEXTA\configs\lidargo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63596D6F-AD9D-4234-AA75-18DE627E4C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5081BE23-45D8-435E-9171-950AEE4D37F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -158,21 +158,12 @@
     <t>sc1.lidar.z01.a0.\d{8}.\d{6}.user4.nc</t>
   </si>
   <si>
-    <t>sa1.lidar.z05.a2.\d{8}.\d{6}.user5.nc</t>
-  </si>
-  <si>
     <t>vol</t>
   </si>
   <si>
-    <t>a2</t>
-  </si>
-  <si>
     <t>vad</t>
   </si>
   <si>
-    <t>sa1.lidar.z05.vad.a2.\d{8}.\d{6}.user5.nc</t>
-  </si>
-  <si>
     <t>sa5.lidar.z03.a0.\d{8}.\d{6}.user5.nc</t>
   </si>
   <si>
@@ -186,6 +177,12 @@
   </si>
   <si>
     <t>sc1.lidar.z02.a0.\d{8}.\d{6}.nc</t>
+  </si>
+  <si>
+    <t>sa1.lidar.z05.a0.\d{8}.\d{6}.user5.nc</t>
+  </si>
+  <si>
+    <t>sa1.lidar.z05.vad.a0.\d{8}.\d{6}.user5.nc</t>
   </si>
 </sst>
 </file>
@@ -639,9 +636,9 @@
   </sheetPr>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="88" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,22 +654,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>40</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -743,16 +740,16 @@
         <v>39</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="F5" s="16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -784,10 +781,10 @@
         <v>29</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>29</v>
@@ -847,7 +844,7 @@
         <v>-3</v>
       </c>
       <c r="D10" s="18">
-        <v>-31</v>
+        <v>-40</v>
       </c>
       <c r="E10" s="18">
         <v>-0.1</v>
@@ -867,7 +864,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="18">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E11" s="18">
         <v>0.1</v>

</xml_diff>